<commit_message>
Added Strings Patterns Excel
</commit_message>
<xml_diff>
--- a/Excel_docs/Untitledspreadsheet.xlsx
+++ b/Excel_docs/Untitledspreadsheet.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{234791DD-FA67-4B21-ADF6-6D0F409EEFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="vb" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Login_Check" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="vb" sheetId="2" r:id="rId2"/>
+    <sheet name="Login_Check" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:C7"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
   <si>
     <t>First Name</t>
   </si>
@@ -179,34 +182,39 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF484C55"/>
       <name val="Roboto"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -214,7 +222,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -224,52 +232,43 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -459,28 +458,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" customWidth="true" width="16.13" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.38" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="47.13" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.25" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="17.88" collapsed="true"/>
+    <col min="4" max="4" width="16.109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="47.109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.21875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -523,10 +525,10 @@
         <v>12</v>
       </c>
       <c r="D2" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2">
-        <v>44964.0</v>
+        <v>44964</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
@@ -544,39 +546,40 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="66.25" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="54.5" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="47.63" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="41.38" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="19.5" collapsed="true"/>
+    <col min="2" max="2" width="66.21875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="54.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="47.6640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="41.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -605,7 +608,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -634,7 +637,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -663,7 +666,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
@@ -694,36 +697,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
-  <drawing r:id="rId4"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.13" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="69.25" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="55.5" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="54.25" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="47.63" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.25" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="23.5" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="42.13" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="23.25" collapsed="true"/>
+    <col min="1" max="1" width="23.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="69.21875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="55.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="54.21875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="47.6640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.21875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.44140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="42.109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.21875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -752,7 +756,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -778,7 +782,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -804,7 +808,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
@@ -832,10 +836,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
   </hyperlinks>
-  <drawing r:id="rId4"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>